<commit_message>
Thêm plan công việc của giang
</commit_message>
<xml_diff>
--- a/hop/log.xlsx
+++ b/hop/log.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\InternAtwoM\project\hop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7168C9DD-9B84-40A3-A5C1-DD6E4CBF2C3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084AF0C1-1E06-4501-9502-31943C08ADFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{78C26181-3197-4AC1-B1A0-F8D659C78093}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{78C26181-3197-4AC1-B1A0-F8D659C78093}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Giang" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Nhóm 2</t>
   </si>
@@ -172,12 +173,57 @@
   </si>
   <si>
     <t>Giải thích cấu trúc thư mục, sửa db và đưa ra các quy chuẩn để code + sửa phần sơ đồ tuần tự</t>
+  </si>
+  <si>
+    <t>Đầu việc</t>
+  </si>
+  <si>
+    <t>Bắt đầu</t>
+  </si>
+  <si>
+    <t>Kết thúc</t>
+  </si>
+  <si>
+    <t>Khởi tạo cấu trúc thư mục BE</t>
+  </si>
+  <si>
+    <t>Viết liquibase</t>
+  </si>
+  <si>
+    <t>Config Security + Jwt</t>
+  </si>
+  <si>
+    <t>Xây dựng api đăng ký đăng nhập</t>
+  </si>
+  <si>
+    <t>Xây dựng giao diện đăng ký đăng nhập</t>
+  </si>
+  <si>
+    <t>Xây dựng dựng service token và interceptor</t>
+  </si>
+  <si>
+    <t>Xây dựng api xem thông tin user</t>
+  </si>
+  <si>
+    <t>Xây dựng page user</t>
+  </si>
+  <si>
+    <t>Xây dựng api sân bóng</t>
+  </si>
+  <si>
+    <t>Xây dựng giao diện sân bóng</t>
+  </si>
+  <si>
+    <t>Xây dựng giao diện chi tiết sân bóng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yy;@"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -231,7 +277,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -266,6 +312,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -583,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E41A48-58C5-48BC-8F73-F4E51E05CF77}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -897,4 +944,157 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64E95BBF-BC24-4502-8852-C3966794EEF4}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="36.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="17.6640625" style="12" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="12"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" s="12">
+        <v>45506</v>
+      </c>
+      <c r="C2" s="12">
+        <v>45507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3" s="12">
+        <v>45508</v>
+      </c>
+      <c r="C3" s="12">
+        <v>45509</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="12">
+        <v>45510</v>
+      </c>
+      <c r="C4" s="12">
+        <v>45511</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="12">
+        <v>45512</v>
+      </c>
+      <c r="C5" s="12">
+        <v>45513</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="12">
+        <v>45514</v>
+      </c>
+      <c r="C6" s="12">
+        <v>45515</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="12">
+        <v>45516</v>
+      </c>
+      <c r="C7" s="12">
+        <v>45517</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="12">
+        <v>45518</v>
+      </c>
+      <c r="C8" s="12">
+        <v>45519</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="12">
+        <v>45520</v>
+      </c>
+      <c r="C9" s="12">
+        <v>45521</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="12">
+        <v>45522</v>
+      </c>
+      <c r="C10" s="12">
+        <v>45523</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="12">
+        <v>45524</v>
+      </c>
+      <c r="C11" s="12">
+        <v>45525</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="12">
+        <v>45526</v>
+      </c>
+      <c r="C12" s="12">
+        <v>45527</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>